<commit_message>
Update .gitignore, modify CORS settings, and enhance Dockerfile for frontend build
</commit_message>
<xml_diff>
--- a/examples/Worked_out_example.xlsx
+++ b/examples/Worked_out_example.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasdebie/mhc_comparison/test_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasdebie/mhcmatchmaker/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DC7981-9557-9D46-9637-B35B57BEDF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F99BCF-C80F-CD4D-B444-B2AF8D139CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31240" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{87043B3B-D488-F348-BBAB-B06267B1BE21}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{87043B3B-D488-F348-BBAB-B06267B1BE21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F36566-3FD4-A44C-B1EB-95573786E87D}">
   <dimension ref="A1:AX38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="166" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,7 +694,18 @@
     <col min="9" max="9" width="16.83203125" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" customWidth="1"/>
     <col min="11" max="11" width="16.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="21.83203125" customWidth="1"/>
     <col min="14" max="14" width="16.33203125" customWidth="1"/>
+    <col min="15" max="15" width="17.83203125" customWidth="1"/>
+    <col min="16" max="16" width="19.5" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" customWidth="1"/>
+    <col min="18" max="18" width="20" customWidth="1"/>
+    <col min="19" max="19" width="22" customWidth="1"/>
+    <col min="20" max="20" width="17.1640625" customWidth="1"/>
+    <col min="21" max="21" width="18.5" customWidth="1"/>
+    <col min="22" max="22" width="18.83203125" customWidth="1"/>
+    <col min="23" max="23" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
@@ -987,123 +998,123 @@
     <row r="7" spans="1:50" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
       <c r="G7" t="str">
-        <f>REPLACE(G6,1,1,"")</f>
+        <f t="shared" ref="G7:AJ7" si="0">REPLACE(G6,1,1,"")</f>
         <v/>
       </c>
       <c r="H7" t="str">
-        <f>REPLACE(H6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I7" t="str">
-        <f>REPLACE(I6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J7" t="str">
-        <f>REPLACE(J6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K7" t="str">
-        <f>REPLACE(K6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L7" t="str">
-        <f>REPLACE(L6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M7" t="str">
-        <f>REPLACE(M6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N7" t="str">
-        <f>REPLACE(N6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="O7" t="str">
-        <f>REPLACE(O6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P7" t="str">
-        <f>REPLACE(P6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q7" t="str">
-        <f>REPLACE(Q6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="R7" t="str">
-        <f>REPLACE(R6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S7" t="str">
-        <f>REPLACE(S6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="T7" t="str">
-        <f>REPLACE(T6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="U7" t="str">
-        <f>REPLACE(U6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="V7" t="str">
-        <f>REPLACE(V6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="W7" t="str">
-        <f>REPLACE(W6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="X7" t="str">
-        <f>REPLACE(X6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Y7" t="str">
-        <f>REPLACE(Y6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Z7" t="str">
-        <f>REPLACE(Z6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="AA7" t="str">
-        <f>REPLACE(AA6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="AB7" t="str">
-        <f>REPLACE(AB6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="AC7" t="str">
-        <f>REPLACE(AC6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="AD7" t="str">
-        <f>REPLACE(AD6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="AE7" t="str">
-        <f>REPLACE(AE6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="AF7" t="str">
-        <f>REPLACE(AF6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="AG7" t="str">
-        <f>REPLACE(AG6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="AH7" t="str">
-        <f>REPLACE(AH6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="AI7" t="str">
-        <f>REPLACE(AI6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="AJ7" t="str">
-        <f>REPLACE(AJ6,1,1,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>

</xml_diff>